<commit_message>
modified:   OJ/tmp/query.py 	new file:   PyTorch/test.ipynb 	modified:   PyTorch/test.py 	deleted:    Python/test3.py 	deleted:    Python/text.txt 	modified:   "Python/\346\231\202\346\225\270\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/Python/時數表.xlsx
+++ b/Python/時數表.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B197429-5238-49CD-8085-B95DBE06A12D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2FA996-42C6-4BAE-AA46-67B8BD31BD1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
+    <t>曾閔歆</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -480,43 +480,119 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="7">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2">
-        <v>50</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>